<commit_message>
Update the data set to add APSIM soil paramenters
</commit_message>
<xml_diff>
--- a/Rice_PADDY_sample/raw/Field_Overlay1 - piped.xlsx
+++ b/Rice_PADDY_sample/raw/Field_Overlay1 - piped.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-48" windowWidth="12492" windowHeight="6996" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-48" windowWidth="12492" windowHeight="6996"/>
   </bookViews>
   <sheets>
     <sheet name="Field_Overlay_all" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="234">
   <si>
     <t>cm</t>
   </si>
@@ -648,6 +648,78 @@
   </si>
   <si>
     <t>PADDY_2</t>
+  </si>
+  <si>
+    <t>Soil water content, air dry</t>
+  </si>
+  <si>
+    <t>Soil water, lower limit</t>
+  </si>
+  <si>
+    <t>SLADR</t>
+  </si>
+  <si>
+    <t>$SLLL</t>
+  </si>
+  <si>
+    <t>APSIM Evaporative diffusion constant</t>
+  </si>
+  <si>
+    <t>DiffusConst</t>
+  </si>
+  <si>
+    <t>APSIM Evaporative diffusion slope</t>
+  </si>
+  <si>
+    <t>DiffusSlope</t>
+  </si>
+  <si>
+    <t>Apsim Cona soil evaporation</t>
+  </si>
+  <si>
+    <t>CONA</t>
+  </si>
+  <si>
+    <t>Summer soil evaporation, upper limit for stage 1</t>
+  </si>
+  <si>
+    <t>SummerU</t>
+  </si>
+  <si>
+    <t>Winter soil evaporation, upper limit for stage 1</t>
+  </si>
+  <si>
+    <t>WinterU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date to switch to SummerU </t>
+  </si>
+  <si>
+    <t>SummerDate__soil</t>
+  </si>
+  <si>
+    <t>03-21</t>
+  </si>
+  <si>
+    <t>Date to switch to WinterU</t>
+  </si>
+  <si>
+    <t>WinterDate__soil</t>
+  </si>
+  <si>
+    <t>09-21</t>
+  </si>
+  <si>
+    <t>APSIM plant specific water uptake coefficient</t>
+  </si>
+  <si>
+    <t>apsim_kl</t>
+  </si>
+  <si>
+    <t>Biologically active soil organic carbon by layer</t>
+  </si>
+  <si>
+    <t>slacc</t>
   </si>
 </sst>
 </file>
@@ -732,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -816,6 +888,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,7 +1196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -3037,7 +3121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -3700,9 +3784,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -4217,9 +4303,394 @@
     <row r="37" spans="1:8">
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="B38" s="5"/>
-      <c r="D38"/>
+    <row r="38" spans="1:8" ht="28.8">
+      <c r="A38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="42">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="24"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="28.8">
+      <c r="A41" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="28">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="24"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="28.8">
+      <c r="A44" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="H44" s="31"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D45" s="28">
+        <v>16</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="24"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="28.8">
+      <c r="A47" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="24"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="43.2">
+      <c r="A50" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="H50" s="31"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D51" s="28">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="24"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="39" customHeight="1">
+      <c r="A53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="H53" s="31"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" s="28">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="24"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="28.8">
+      <c r="A56" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="H56" s="31"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="24"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="39" customHeight="1">
+      <c r="A59" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="H59" s="31"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="24"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="43.2">
+      <c r="A62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="H62" s="31"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="28">
+        <v>0.06</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="24"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="28.8">
+      <c r="A65" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="H65" s="31"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4229,9 +4700,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -4746,9 +5219,394 @@
     <row r="37" spans="1:8">
       <c r="B37"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="B38" s="5"/>
-      <c r="D38"/>
+    <row r="38" spans="1:8" ht="28.8">
+      <c r="A38" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="42">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="24"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="28.8">
+      <c r="A41" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" s="28">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="24"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="28.8">
+      <c r="A44" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="H44" s="31"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D45" s="28">
+        <v>16</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="24"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="28.8">
+      <c r="A47" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="24"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="43.2">
+      <c r="A50" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="H50" s="31"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D51" s="28">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="24"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="39" customHeight="1">
+      <c r="A53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="H53" s="31"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" s="28">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="24"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="28.8">
+      <c r="A56" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="H56" s="31"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="24"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="39" customHeight="1">
+      <c r="A59" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="H59" s="31"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>229</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="24"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="43.2">
+      <c r="A62" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="H62" s="31"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="28">
+        <v>0.06</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="24"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="28.8">
+      <c r="A65" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="H65" s="31"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>